<commit_message>
Curva de caracterización del Sharp
</commit_message>
<xml_diff>
--- a/Motores/CaracterizacionSharp.xlsx
+++ b/Motores/CaracterizacionSharp.xlsx
@@ -4,13 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="10008" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="10008"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="Hoja1 (2)" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="144525" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -463,11 +463,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="198230016"/>
-        <c:axId val="198231936"/>
+        <c:axId val="195992576"/>
+        <c:axId val="135705344"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="198230016"/>
+        <c:axId val="195992576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -513,6 +513,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -557,12 +558,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="198231936"/>
+        <c:crossAx val="135705344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="198231936"/>
+        <c:axId val="135705344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -665,7 +666,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="198230016"/>
+        <c:crossAx val="195992576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -732,6 +733,22 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" vert="horz"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Curva de Caracterización del Sharp</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -740,26 +757,6 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -768,10 +765,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="8.670603674540682E-2"/>
+          <c:x val="0.12944112154249948"/>
           <c:y val="0.14856481481481484"/>
-          <c:w val="0.87762729658792649"/>
-          <c:h val="0.72088764946048411"/>
+          <c:w val="0.8348921529039639"/>
+          <c:h val="0.68820809163560448"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -1087,16 +1084,35 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="147994112"/>
-        <c:axId val="148017536"/>
+        <c:axId val="41030016"/>
+        <c:axId val="135719552"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="147994112"/>
+        <c:axId val="41030016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Distancia, d (cm)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1115,36 +1131,54 @@
           <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:bodyPr rot="-60000000" vert="horz"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
+              <a:defRPr sz="800"/>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="148017536"/>
+        <c:crossAx val="135719552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="148017536"/>
+        <c:axId val="135719552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="2"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Voltaje, V (v)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="2.4088094757386092E-2"/>
+              <c:y val="0.36962953160266732"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1163,26 +1197,16 @@
           <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:bodyPr rot="-60000000" vert="horz"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
+              <a:defRPr sz="800"/>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="147994112"/>
+        <c:crossAx val="41030016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1218,7 +1242,11 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr/>
+        <a:defRPr sz="1200">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:defRPr>
       </a:pPr>
       <a:endParaRPr lang="en-US"/>
     </a:p>
@@ -1602,11 +1630,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="147891712"/>
-        <c:axId val="147893632"/>
+        <c:axId val="41081088"/>
+        <c:axId val="41251200"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="147891712"/>
+        <c:axId val="41081088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1697,12 +1725,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="147893632"/>
+        <c:crossAx val="41251200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="147893632"/>
+        <c:axId val="41251200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1805,7 +1833,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="147891712"/>
+        <c:crossAx val="41081088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1955,11 +1983,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="136963968"/>
-        <c:axId val="136962432"/>
+        <c:axId val="41554688"/>
+        <c:axId val="41556224"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="136963968"/>
+        <c:axId val="41554688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1969,12 +1997,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="136962432"/>
+        <c:crossAx val="41556224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="136962432"/>
+        <c:axId val="41556224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1984,7 +2012,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="136963968"/>
+        <c:crossAx val="41554688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2388,7 +2416,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2398,8 +2426,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B42" sqref="B42"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J45" sqref="J45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2722,7 +2750,7 @@
         <v>0.36</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
         <v>70</v>
       </c>
@@ -2730,7 +2758,7 @@
         <v>0.32</v>
       </c>
     </row>
-    <row r="41" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
         <v>75</v>
       </c>
@@ -2764,7 +2792,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -3064,7 +3092,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
         <v>55</v>
       </c>
@@ -3072,7 +3100,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="38" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
         <v>60</v>
       </c>
@@ -3080,7 +3108,7 @@
         <v>0.36</v>
       </c>
     </row>
-    <row r="39" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
         <v>65</v>
       </c>

</xml_diff>